<commit_message>
Left adjust equations and general formatting
</commit_message>
<xml_diff>
--- a/Corrections/Corrections Response.xlsx
+++ b/Corrections/Corrections Response.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\PhDThesis\Corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF46436-0DF7-4386-9BAF-3F5E9A54C893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4296B79D-6205-47F1-A647-9EEEC6249C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
   </bookViews>
   <sheets>
     <sheet name="Tom Slatter + Amir Kadiric" sheetId="1" r:id="rId1"/>
+    <sheet name="Additional Corrections" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
   <si>
     <t>Section</t>
   </si>
@@ -444,6 +445,12 @@
   </si>
   <si>
     <t>Did not use Gupta corrections for this</t>
+  </si>
+  <si>
+    <t>Left adjust equations</t>
+  </si>
+  <si>
+    <t>Mofidifed graphics</t>
   </si>
 </sst>
 </file>
@@ -513,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -535,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F42DE2-BF3F-4B4A-ACA4-1B57B73DE292}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -930,7 +934,7 @@
       <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="6"/>
       <c r="E3" s="2">
         <v>5</v>
@@ -2249,4 +2253,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EBFB04-0F62-47B7-B09C-A1466178A0DF}">
+  <dimension ref="B2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aims and objectives (draft), function of RB, Hertz theory, tribofilms, starvation, SRR
</commit_message>
<xml_diff>
--- a/Corrections/Corrections Response.xlsx
+++ b/Corrections/Corrections Response.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\PhDThesis\Corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4296B79D-6205-47F1-A647-9EEEC6249C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1781B2DC-A223-41E0-A230-A405703DA466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
   </bookViews>
   <sheets>
     <sheet name="Tom Slatter + Amir Kadiric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="143">
   <si>
     <t>Section</t>
   </si>
@@ -165,9 +165,6 @@
     <t>No change</t>
   </si>
   <si>
-    <t>Add AVL to reference</t>
-  </si>
-  <si>
     <t>Model from AVL Resbox</t>
   </si>
   <si>
@@ -201,27 +198,15 @@
     <t>Concave, convex and flat</t>
   </si>
   <si>
-    <t>Add "typically" for machine components</t>
-  </si>
-  <si>
     <t>Conformal contact pressures can be regarded as low pressure</t>
   </si>
   <si>
-    <t>Clear order of magnitudes</t>
-  </si>
-  <si>
     <t>Both convex not true for ball bearing</t>
   </si>
   <si>
-    <t>Clarify the types of contact</t>
-  </si>
-  <si>
     <t>It is either elliptical or point, not both</t>
   </si>
   <si>
-    <t>Clarify</t>
-  </si>
-  <si>
     <t>State main assumptions in Hertz theory</t>
   </si>
   <si>
@@ -243,9 +228,6 @@
     <t>For accurate predictions (including bearing life predictions) none of this is used, but a full numerical contact model is used instead, which can even include roughness and asperity stress history. I think you need to update the text to clarify this</t>
   </si>
   <si>
-    <t>Only for SKF GLBM. Clarify in text that I refer to MBD modelling.</t>
-  </si>
-  <si>
     <t>Typical EHL pressures in "steel contacts"</t>
   </si>
   <si>
@@ -264,9 +246,6 @@
     <t>How/why does starvation occur in bearings? Explain briefly</t>
   </si>
   <si>
-    <t>Cavitation and lack of replenishment</t>
-  </si>
-  <si>
     <t>What are the typical SRR in bearings? Very small 2-5% in most cases. up to 10-15% in specific bearings, thrust roller bearings for example</t>
   </si>
   <si>
@@ -297,9 +276,6 @@
     <t>Clarify if rig was partly/entirely built by candidate</t>
   </si>
   <si>
-    <t>Twas all me</t>
-  </si>
-  <si>
     <t>What acceleration is this from 0-15000rpm in 4s? Was this accounted for in the EHL film predictions? What entrainment speed? Are there inlet shear heating effects? You go through a lot of trouble to describe the 1D Reynolds solver but these other factors may be just as (or even more) important. Add brief discussion.</t>
   </si>
   <si>
@@ -451,13 +427,52 @@
   </si>
   <si>
     <t>Mofidifed graphics</t>
+  </si>
+  <si>
+    <t>Did not cite</t>
+  </si>
+  <si>
+    <t>As above</t>
+  </si>
+  <si>
+    <t>Addressed by restructuring with clearer defintions of aims and objectives. Added Scope of Research and Tasks.</t>
+  </si>
+  <si>
+    <t>Clarified to state that the significant difference in radii and rephrased.</t>
+  </si>
+  <si>
+    <t>Ammended</t>
+  </si>
+  <si>
+    <t>Noted similar radii and added flat</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Mechanism explained in 2.4.3 Starvation. Refined.</t>
+  </si>
+  <si>
+    <t>Rephrased to deform within small-strain (linear elastic)</t>
+  </si>
+  <si>
+    <t>Did not elaborate</t>
+  </si>
+  <si>
+    <t>Assumptions stated</t>
+  </si>
+  <si>
+    <t>Clarified. Cylinders have finite length, no infinitely long cylinders. Therefore adjustment required to capture edge effects</t>
+  </si>
+  <si>
+    <t>Added note on computationally efficient models that can be used in dynamic solvers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,8 +508,22 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +536,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -517,10 +556,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -543,8 +584,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -879,15 +937,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F42DE2-BF3F-4B4A-ACA4-1B57B73DE292}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="80" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
@@ -966,8 +1024,10 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E5" s="2">
         <v>4</v>
       </c>
@@ -980,8 +1040,10 @@
       <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
@@ -996,7 +1058,9 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2">
         <v>3</v>
@@ -1024,7 +1088,9 @@
       <c r="B9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2">
         <v>1</v>
@@ -1038,10 +1104,10 @@
       <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -1056,7 +1122,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
@@ -1070,7 +1136,7 @@
       <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1114,11 +1180,11 @@
     <row r="15" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -1130,11 +1196,11 @@
     <row r="16" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -1146,11 +1212,11 @@
     <row r="17" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -1162,7 +1228,7 @@
     <row r="18" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
@@ -1176,11 +1242,11 @@
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
@@ -1192,12 +1258,12 @@
     <row r="20" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="2">
         <v>4</v>
       </c>
@@ -1208,14 +1274,12 @@
     <row r="21" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="2">
         <v>1</v>
       </c>
@@ -1226,12 +1290,12 @@
     <row r="22" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="2">
         <v>4</v>
       </c>
@@ -1242,12 +1306,12 @@
     <row r="23" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="2">
         <v>4</v>
       </c>
@@ -1258,9 +1322,11 @@
     <row r="24" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>140</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2">
         <v>4</v>
@@ -1272,9 +1338,11 @@
     <row r="25" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>139</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2">
         <v>1</v>
@@ -1286,11 +1354,13 @@
     <row r="26" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
@@ -1302,11 +1372,13 @@
     <row r="27" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>141</v>
+      </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E27" s="2">
         <v>3</v>
@@ -1318,12 +1390,12 @@
     <row r="28" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="2">
         <v>2</v>
       </c>
@@ -1334,12 +1406,12 @@
     <row r="29" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="2">
         <v>4</v>
       </c>
@@ -1350,12 +1422,12 @@
     <row r="30" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="2">
         <v>4</v>
       </c>
@@ -1366,11 +1438,11 @@
     <row r="31" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
@@ -1382,12 +1454,12 @@
     <row r="32" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="2">
         <v>4</v>
       </c>
@@ -1398,9 +1470,11 @@
     <row r="33" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2">
         <v>4</v>
@@ -1412,7 +1486,7 @@
     <row r="34" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="1"/>
@@ -1426,7 +1500,7 @@
     <row r="35" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="1"/>
@@ -1440,12 +1514,12 @@
     <row r="36" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2">
         <v>2</v>
       </c>
@@ -1480,7 +1554,7 @@
     <row r="39" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="1"/>
@@ -1494,11 +1568,11 @@
     <row r="40" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -1510,7 +1584,7 @@
     <row r="41" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="1"/>
@@ -1524,11 +1598,11 @@
     <row r="42" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -1540,12 +1614,10 @@
     <row r="43" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="2">
         <v>4</v>
       </c>
@@ -1556,11 +1628,11 @@
     <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E44" s="2">
         <v>3</v>
@@ -1572,11 +1644,11 @@
     <row r="45" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E45" s="2">
         <v>4</v>
@@ -1588,11 +1660,11 @@
     <row r="46" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
@@ -1604,11 +1676,11 @@
     <row r="47" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="C47" s="8"/>
       <c r="D47" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E47" s="2">
         <v>3</v>
@@ -1620,11 +1692,11 @@
     <row r="48" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E48" s="2">
         <v>3</v>
@@ -1636,11 +1708,11 @@
     <row r="49" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -1652,11 +1724,11 @@
     <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E50" s="2">
         <v>3</v>
@@ -1668,11 +1740,11 @@
     <row r="51" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E51" s="2">
         <v>4</v>
@@ -1684,7 +1756,7 @@
     <row r="52" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="1"/>
@@ -1698,7 +1770,7 @@
     <row r="53" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
@@ -1712,11 +1784,11 @@
     <row r="54" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E54" s="2">
         <v>4</v>
@@ -1783,7 +1855,7 @@
     <row r="59" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="1"/>
@@ -1797,7 +1869,7 @@
     <row r="60" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
@@ -1827,7 +1899,7 @@
     <row r="62" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="1"/>
@@ -1841,11 +1913,11 @@
     <row r="63" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E63" s="2">
         <v>3</v>
@@ -1857,7 +1929,7 @@
     <row r="64" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="1"/>
@@ -1871,7 +1943,7 @@
     <row r="65" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="1"/>
@@ -1885,11 +1957,11 @@
     <row r="66" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E66" s="2">
         <v>3</v>
@@ -1901,7 +1973,7 @@
     <row r="67" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1"/>
@@ -1915,11 +1987,11 @@
     <row r="68" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E68" s="2">
         <v>2</v>
@@ -1949,7 +2021,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E70" s="2">
         <v>2</v>
@@ -1989,7 +2061,7 @@
     <row r="73" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="1"/>
@@ -2019,7 +2091,7 @@
     <row r="75" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="7" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="1"/>
@@ -2033,7 +2105,7 @@
     <row r="76" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="1"/>
@@ -2047,11 +2119,11 @@
     <row r="77" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E77" s="2">
         <v>4</v>
@@ -2063,11 +2135,11 @@
     <row r="78" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E78" s="2">
         <v>4</v>
@@ -2079,11 +2151,11 @@
     <row r="79" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E79" s="2">
         <v>1</v>
@@ -2095,11 +2167,11 @@
     <row r="80" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E80" s="2">
         <v>1</v>
@@ -2111,11 +2183,11 @@
     <row r="81" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E81" s="2">
         <v>3</v>
@@ -2127,7 +2199,7 @@
     <row r="82" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="1"/>
@@ -2141,11 +2213,11 @@
     <row r="83" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E83" s="2">
         <v>3</v>
@@ -2157,11 +2229,11 @@
     <row r="84" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E84" s="2">
         <v>3</v>
@@ -2173,7 +2245,7 @@
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="1"/>
@@ -2217,11 +2289,11 @@
     <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E88" s="2">
         <v>3</v>
@@ -2259,7 +2331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EBFB04-0F62-47B7-B09C-A1466178A0DF}">
   <dimension ref="B2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -2270,12 +2342,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Literature review, short experimental, short FMBD
</commit_message>
<xml_diff>
--- a/Corrections/Corrections Response.xlsx
+++ b/Corrections/Corrections Response.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\PhDThesis\Corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1781B2DC-A223-41E0-A230-A405703DA466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD04E42-C510-4D19-BF68-68F84964EC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4546FF8B-BC23-429E-85B6-7F6A0D840A61}"/>
   </bookViews>
   <sheets>
     <sheet name="Tom Slatter + Amir Kadiric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="156">
   <si>
     <t>Section</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Contact pressures for 750 N loaded case</t>
   </si>
   <si>
-    <t>Discuss what is considered high-speed in relation to automotive</t>
-  </si>
-  <si>
     <t>Accuracy of displacement measurements</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>Remove shear strength of asperities and specific heat capacity of solids</t>
   </si>
   <si>
-    <t>Small ammendment. Explain not required.</t>
-  </si>
-  <si>
     <t>Improve description of figure 3.13</t>
   </si>
   <si>
@@ -351,9 +345,6 @@
     <t xml:space="preserve">OK. How does this value compare to that from simple EHD regression predictions? </t>
   </si>
   <si>
-    <t>Same comment as above</t>
-  </si>
-  <si>
     <t>Comment on the significane of the huge increase in contact force</t>
   </si>
   <si>
@@ -381,9 +372,6 @@
     <t>How did you determine 9 input variables?</t>
   </si>
   <si>
-    <t>Relevant variables for the EHL film thickness calculation.</t>
-  </si>
-  <si>
     <t>Clarify difference between Greenwood boundary this approach and Marian.</t>
   </si>
   <si>
@@ -466,6 +454,57 @@
   </si>
   <si>
     <t>Added note on computationally efficient models that can be used in dynamic solvers.</t>
+  </si>
+  <si>
+    <t>Reordered</t>
+  </si>
+  <si>
+    <t>Added to subsection 2.1.2 at start of Lit Review</t>
+  </si>
+  <si>
+    <t>Clarified analytical dynamic models, then commented on advancement to couple tribo-dynamic modelling</t>
+  </si>
+  <si>
+    <t>Finite length line contact, cited Hertz (1881) and Johnson (1985)</t>
+  </si>
+  <si>
+    <t>Corrected.</t>
+  </si>
+  <si>
+    <t>Removed, these are from a previous paper and not relevant to the current work</t>
+  </si>
+  <si>
+    <t>Done and amended another</t>
+  </si>
+  <si>
+    <t>Required variables for the EHL film thickness calculation.</t>
+  </si>
+  <si>
+    <t>Added section 2.1.3 to Literature Raeview under "Characterisatin of High-Speed Bearings"</t>
+  </si>
+  <si>
+    <t>Added nDm value. Discussion on what is considered high-speed is now included in new section 2.1.3 in literature review</t>
+  </si>
+  <si>
+    <t>Contact pressures are presented in the results section, and vary depending on dynamic response of rig (eg. resonance). A single nominal value would not be representative here.</t>
+  </si>
+  <si>
+    <t>Added in a footnote</t>
+  </si>
+  <si>
+    <t>Added reference to film acting as interference wedge at the start of section and made the description clearer to reflect what was discussed in the viva.</t>
+  </si>
+  <si>
+    <t>Contact oscillation and change of regime explained in the text as discussed in the viva.</t>
+  </si>
+  <si>
+    <t>Clarified as maximum average torque of 68Nm in the constant torque region</t>
+  </si>
+  <si>
+    <t>Full landscape page</t>
+  </si>
+  <si>
+    <t>This is already explained in section 4.3.2, including what isn't modelled (flexible bodies in representative excitation model and stator tooth forces duer to minimal lateral contribution once resolved).</t>
   </si>
 </sst>
 </file>
@@ -561,7 +600,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -585,9 +624,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
@@ -595,9 +631,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -937,15 +970,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F42DE2-BF3F-4B4A-ACA4-1B57B73DE292}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="80" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
@@ -1024,10 +1057,10 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="C5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="2">
         <v>4</v>
       </c>
@@ -1040,10 +1073,10 @@
       <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="C6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="2">
         <v>4</v>
       </c>
@@ -1058,8 +1091,8 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>136</v>
+      <c r="C7" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2">
@@ -1074,7 +1107,9 @@
       <c r="B8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="2">
         <v>2</v>
@@ -1088,8 +1123,8 @@
       <c r="B9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>130</v>
+      <c r="C9" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2">
@@ -1104,8 +1139,8 @@
       <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>136</v>
+      <c r="C10" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="2">
@@ -1136,7 +1171,7 @@
       <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1154,7 +1189,9 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <v>4</v>
@@ -1168,7 +1205,9 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="9" t="s">
+        <v>139</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2">
         <v>3</v>
@@ -1230,7 +1269,9 @@
       <c r="B18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2">
         <v>5</v>
@@ -1260,8 +1301,8 @@
       <c r="B20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>135</v>
+      <c r="C20" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2">
@@ -1276,8 +1317,8 @@
       <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>134</v>
+      <c r="C21" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2">
@@ -1292,8 +1333,8 @@
       <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>133</v>
+      <c r="C22" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2">
@@ -1308,8 +1349,8 @@
       <c r="B23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>134</v>
+      <c r="C23" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2">
@@ -1324,8 +1365,8 @@
       <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>140</v>
+      <c r="C24" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2">
@@ -1340,8 +1381,8 @@
       <c r="B25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>139</v>
+      <c r="C25" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2">
@@ -1356,8 +1397,8 @@
       <c r="B26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>138</v>
+      <c r="C26" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>58</v>
@@ -1374,8 +1415,8 @@
       <c r="B27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>141</v>
+      <c r="C27" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>61</v>
@@ -1392,8 +1433,8 @@
       <c r="B28" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>142</v>
+      <c r="C28" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2">
@@ -1408,8 +1449,8 @@
       <c r="B29" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>134</v>
+      <c r="C29" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
@@ -1424,8 +1465,8 @@
       <c r="B30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>134</v>
+      <c r="C30" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2">
@@ -1456,8 +1497,8 @@
       <c r="B32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>137</v>
+      <c r="C32" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2">
@@ -1472,8 +1513,8 @@
       <c r="B33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>136</v>
+      <c r="C33" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2">
@@ -1516,8 +1557,8 @@
       <c r="B36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>136</v>
+      <c r="C36" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2">
@@ -1556,7 +1597,9 @@
       <c r="B39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="2">
         <v>2</v>
@@ -1568,12 +1611,12 @@
     <row r="40" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="2">
         <v>2</v>
       </c>
@@ -1584,7 +1627,7 @@
     <row r="41" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="1"/>
@@ -1598,11 +1641,11 @@
     <row r="42" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -1614,9 +1657,11 @@
     <row r="43" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2">
         <v>4</v>
@@ -1628,11 +1673,11 @@
     <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="2">
         <v>3</v>
@@ -1644,9 +1689,11 @@
     <row r="45" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1660,9 +1707,11 @@
     <row r="46" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>64</v>
       </c>
@@ -1676,9 +1725,11 @@
     <row r="47" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="D47" s="1" t="s">
         <v>64</v>
       </c>
@@ -1692,11 +1743,11 @@
     <row r="48" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E48" s="2">
         <v>3</v>
@@ -1708,11 +1759,11 @@
     <row r="49" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -1724,11 +1775,11 @@
     <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" s="2">
         <v>3</v>
@@ -1740,12 +1791,12 @@
     <row r="51" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="2">
         <v>4</v>
       </c>
@@ -1756,9 +1807,11 @@
     <row r="52" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>152</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2">
         <v>3</v>
@@ -1770,9 +1823,11 @@
     <row r="53" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2">
         <v>3</v>
@@ -1784,12 +1839,12 @@
     <row r="54" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="2">
         <v>4</v>
       </c>
@@ -1855,7 +1910,7 @@
     <row r="59" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="1"/>
@@ -1869,7 +1924,7 @@
     <row r="60" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
@@ -1899,7 +1954,7 @@
     <row r="62" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="1"/>
@@ -1913,12 +1968,12 @@
     <row r="63" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" s="1"/>
       <c r="E63" s="2">
         <v>3</v>
       </c>
@@ -1929,7 +1984,7 @@
     <row r="64" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="1"/>
@@ -1943,9 +1998,11 @@
     <row r="65" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="2">
         <v>3</v>
@@ -1957,11 +2014,11 @@
     <row r="66" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E66" s="2">
         <v>3</v>
@@ -1973,7 +2030,7 @@
     <row r="67" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1"/>
@@ -1987,12 +2044,10 @@
     <row r="68" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="D68" s="1"/>
       <c r="E68" s="2">
         <v>2</v>
       </c>
@@ -2005,7 +2060,9 @@
       <c r="B69" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C69" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69" s="2">
         <v>2</v>
@@ -2021,7 +2078,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E70" s="2">
         <v>2</v>
@@ -2035,7 +2092,9 @@
       <c r="B71" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="2"/>
+      <c r="C71" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71" s="2">
         <v>4</v>
@@ -2061,7 +2120,7 @@
     <row r="73" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="1"/>
@@ -2091,7 +2150,7 @@
     <row r="75" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="1"/>
@@ -2105,7 +2164,7 @@
     <row r="76" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="1"/>
@@ -2119,11 +2178,11 @@
     <row r="77" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E77" s="2">
         <v>4</v>
@@ -2135,11 +2194,11 @@
     <row r="78" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E78" s="2">
         <v>4</v>
@@ -2151,11 +2210,13 @@
     <row r="79" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="D79" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="E79" s="2">
         <v>1</v>
@@ -2167,11 +2228,13 @@
     <row r="80" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C80" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="D80" s="1" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="E80" s="2">
         <v>1</v>
@@ -2183,11 +2246,11 @@
     <row r="81" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E81" s="2">
         <v>3</v>
@@ -2199,7 +2262,7 @@
     <row r="82" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="1"/>
@@ -2213,11 +2276,11 @@
     <row r="83" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E83" s="2">
         <v>3</v>
@@ -2229,11 +2292,11 @@
     <row r="84" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E84" s="2">
         <v>3</v>
@@ -2245,7 +2308,7 @@
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="1"/>
@@ -2286,15 +2349,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D88" s="1"/>
       <c r="E88" s="2">
         <v>3</v>
       </c>
@@ -2342,12 +2405,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>